<commit_message>
near full: problem with encode
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ami05\Desktop\develop\back-end\exselScriptSSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{582BF954-E808-46B5-8626-5B6DFC682837}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43C10CC-E06A-46E3-8697-B7535377A02B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3585" windowWidth="21600" windowHeight="11310" xr2:uid="{1CF26472-2DA0-4F1F-A49C-FFDEFA4FAF19}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>фамилия</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>А хз вообще</t>
+  </si>
+  <si>
+    <t>holod</t>
+  </si>
+  <si>
+    <t>data</t>
   </si>
 </sst>
 </file>
@@ -418,11 +424,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0533768-2208-458B-BEF2-6C5C24119CD0}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -500,6 +504,23 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>322</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>